<commit_message>
change paths and names, add std in single survey codes
</commit_message>
<xml_diff>
--- a/standard_formats/fishglob_data_columns.xlsx
+++ b/standard_formats/fishglob_data_columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auroremaureaud/Documents/FISHGLOB/integrated_fishglob_surveys/standard_formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4811AC-DBF7-8240-9457-DB3C09AE11D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6054BFE-68F1-5749-BA77-01F81F0A90ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
   <si>
     <t>Column name fishglob</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>wgt_cpua</t>
+  </si>
+  <si>
+    <t>survey_unit</t>
+  </si>
+  <si>
+    <t>combination of survey with quarter or season (useful for BITS, NS-IBTS, SWC-IBTS, NEUS, SEUS, SCS, GMEX)</t>
   </si>
 </sst>
 </file>
@@ -591,10 +597,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1107,6 +1113,17 @@
         <v>90</v>
       </c>
     </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" location="gid=0" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
fix unit of wgt_cpue
</commit_message>
<xml_diff>
--- a/standard_formats/fishglob_data_columns.xlsx
+++ b/standard_formats/fishglob_data_columns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auroremaureaud/Documents/FISHGLOB/integrated_fishglob_surveys/standard_formats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auroremaureaud/Documents/FISHGLOB/FishGlob_data/standard_formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6054BFE-68F1-5749-BA77-01F81F0A90ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75AEC0D-7CA2-FC48-A08F-9EB7BCFE6886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -305,9 +305,6 @@
     <t>Worms rank</t>
   </si>
   <si>
-    <t>kg/min</t>
-  </si>
-  <si>
     <t>degrees, Geographic Coordinate System, WGS84</t>
   </si>
   <si>
@@ -339,13 +336,16 @@
   </si>
   <si>
     <t>combination of survey with quarter or season (useful for BITS, NS-IBTS, SWC-IBTS, NEUS, SEUS, SCS, GMEX)</t>
+  </si>
+  <si>
+    <t>kg/hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -355,6 +355,12 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -377,8 +383,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +607,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -636,24 +643,24 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -793,7 +800,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
@@ -807,7 +814,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
@@ -821,7 +828,7 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
@@ -916,7 +923,7 @@
         <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
@@ -927,7 +934,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
         <v>60</v>
@@ -957,8 +964,8 @@
       <c r="A29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
-        <v>91</v>
+      <c r="B29" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>33</v>
@@ -969,9 +976,9 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C30" t="s">
@@ -1115,13 +1122,13 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
         <v>101</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>